<commit_message>
Commiting work from the last week.
</commit_message>
<xml_diff>
--- a/flint_scripts/BCM Inventory.xlsx
+++ b/flint_scripts/BCM Inventory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
   <si>
     <t>miroc5/rcp26</t>
   </si>
@@ -127,15 +127,6 @@
   </si>
   <si>
     <t>The model that are marked as complete also have the monthly transient data.</t>
-  </si>
-  <si>
-    <t>(Running Python Monthlies)</t>
-  </si>
-  <si>
-    <t>(Copying Monthlies)</t>
-  </si>
-  <si>
-    <t>Copying Monthlies)</t>
   </si>
 </sst>
 </file>
@@ -973,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E9" sqref="E9:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -987,25 +978,25 @@
     <col min="4" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1">
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1">
+    <row r="3" spans="1:4" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1"/>
-    <row r="5" spans="1:5" s="1" customFormat="1"/>
-    <row r="6" spans="1:5" s="1" customFormat="1"/>
-    <row r="7" spans="1:5" s="1" customFormat="1">
+    <row r="4" spans="1:4" s="1" customFormat="1"/>
+    <row r="5" spans="1:4" s="1" customFormat="1"/>
+    <row r="6" spans="1:4" s="1" customFormat="1"/>
+    <row r="7" spans="1:4" s="1" customFormat="1">
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1016,7 +1007,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1030,7 +1021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1043,11 +1034,8 @@
       <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +1049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1074,11 +1062,8 @@
       <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1091,11 +1076,8 @@
       <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1108,11 +1090,8 @@
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1126,7 +1105,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1140,7 +1119,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
A few changtes to ncml for bcca
</commit_message>
<xml_diff>
--- a/flint_scripts/BCM Inventory.xlsx
+++ b/flint_scripts/BCM Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="27960" yWindow="6360" windowWidth="15600" windowHeight="11640"/>
+    <workbookView xWindow="9020" yWindow="2640" windowWidth="15600" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="CA_T6_BCM" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
   <si>
     <t>miroc5/rcp26</t>
   </si>
@@ -127,13 +127,16 @@
   </si>
   <si>
     <t>The model that are marked as complete also have the monthly transient data.</t>
+  </si>
+  <si>
+    <t>Transferred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +275,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -574,7 +593,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -617,13 +636,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -652,11 +673,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -964,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -976,27 +999,28 @@
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="3" max="3" width="21.1640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+    <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
+    <row r="3" spans="1:5" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="1" customFormat="1"/>
-    <row r="5" spans="1:4" s="1" customFormat="1"/>
-    <row r="6" spans="1:4" s="1" customFormat="1"/>
-    <row r="7" spans="1:4" s="1" customFormat="1">
+    <row r="4" spans="1:5" s="1" customFormat="1"/>
+    <row r="5" spans="1:5" s="1" customFormat="1"/>
+    <row r="6" spans="1:5" s="1" customFormat="1"/>
+    <row r="7" spans="1:5" s="1" customFormat="1">
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1007,7 +1031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1021,7 +1045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1034,8 +1058,11 @@
       <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1048,8 +1075,11 @@
       <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1062,8 +1092,11 @@
       <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1077,7 +1110,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1090,8 +1123,11 @@
       <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1104,8 +1140,11 @@
       <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1118,8 +1157,11 @@
       <c r="D15" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1132,8 +1174,11 @@
       <c r="D16" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1146,8 +1191,11 @@
       <c r="D17" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -1161,7 +1209,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1175,7 +1223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1189,7 +1237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1203,7 +1251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1217,7 +1265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1279,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1245,7 +1293,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -1259,7 +1307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -1272,8 +1320,11 @@
       <c r="D26" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>17</v>
       </c>
@@ -1287,15 +1338,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
@@ -1303,7 +1354,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1311,7 +1362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1324,6 +1375,7 @@
     <sortCondition ref="A3:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>